<commit_message>
DOCUMENTS - TPI transmission du mardi 27- ajout des dernières versions de documents relatifs au TPI
</commit_message>
<xml_diff>
--- a/_Documents_TPI/Plan de test.xlsx
+++ b/_Documents_TPI/Plan de test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://firstpointch-my.sharepoint.com/personal/fscheibler_firstpoint_ch/Documents/TPI_OD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sites\TPI\_Documents_TPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_AD4D9D64A577C15A4A541810909841D45ADEDD89" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6394C0B6-F1D5-4F4B-8667-F16EDFD7C1A1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CAE56B-1426-4562-A099-D9DACE4DB10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="3360" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="109">
   <si>
     <t>Phase</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Configuration de l'environnement avec PHP 8.2</t>
   </si>
   <si>
-    <t>ok</t>
-  </si>
-  <si>
     <t>Exécuter php -v dans le terminal et vérifier que la version retournée est 8.2.</t>
   </si>
   <si>
@@ -349,6 +346,12 @@
   </si>
   <si>
     <t>Les ajustements et nouvelles fonctionnalités fonctionnent comme prévu, sans effets secondaires indésirables.</t>
+  </si>
+  <si>
+    <t>succès immédiat</t>
+  </si>
+  <si>
+    <t>succès après corrections</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -417,16 +423,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ADE18A50-8206-4C71-B1B7-3D84CB848239}" name="Tableau2" displayName="Tableau2" ref="A1:G36" totalsRowShown="0">
-  <autoFilter ref="A1:G36" xr:uid="{ADE18A50-8206-4C71-B1B7-3D84CB848239}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D4A1F4B8-209B-491C-A1CB-6EAD4C876563}" name="Tableau23" displayName="Tableau23" ref="A1:G36" totalsRowShown="0">
+  <autoFilter ref="A1:G36" xr:uid="{D4A1F4B8-209B-491C-A1CB-6EAD4C876563}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{363167EA-A80E-45C6-8F69-930C358904A1}" name="Phase" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{7F82BFB1-D69C-4AEB-936F-2AB338297816}" name="No"/>
-    <tableColumn id="3" xr3:uid="{E065CCA2-E813-4194-8E1A-94A152DCC282}" name="Titre"/>
-    <tableColumn id="4" xr3:uid="{3A47CF8B-5FE9-4D58-BA1D-6139142F6204}" name="Statut"/>
-    <tableColumn id="5" xr3:uid="{4A93CF95-712D-4548-B15E-41BA74F04473}" name="Procédure" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{1DB138AA-0B3A-4C4B-9522-C64032939B84}" name="Critère de réussite" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{B37F13E1-239B-4D68-A179-8CB545227DD1}" name="Remarques"/>
+    <tableColumn id="1" xr3:uid="{F132216B-37DE-48A6-B6F3-BBBA5A6B0428}" name="Phase" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{36A9C71A-55FC-4D2F-9032-AB95A02096F6}" name="No"/>
+    <tableColumn id="3" xr3:uid="{9C3C5BF1-26CF-41C4-94AA-9142BFD66C4C}" name="Titre"/>
+    <tableColumn id="4" xr3:uid="{AE54EBAB-A25E-422D-AC0E-BBA90A4ED657}" name="Statut" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{14462EC1-4377-4C0F-BDFF-0F428C715A2C}" name="Procédure" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{2170F71C-BC14-4394-8843-FBDDD998CAA2}" name="Critère de réussite" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{5590D142-D13A-43D4-8FB4-3F68E21DAB1F}" name="Remarques"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -706,7 +712,7 @@
     <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="79.6328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="75" style="1" customWidth="1"/>
     <col min="7" max="7" width="40.7265625" bestFit="1" customWidth="1"/>
@@ -722,7 +728,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -735,7 +741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2.1</v>
       </c>
@@ -745,17 +751,17 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2.1</v>
       </c>
@@ -763,19 +769,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -786,16 +792,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -806,16 +812,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -826,19 +832,19 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.2000000000000002</v>
       </c>
@@ -846,16 +852,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -866,13 +872,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -883,13 +892,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -900,13 +912,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -917,13 +932,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -934,13 +952,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -951,13 +972,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -968,13 +992,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -985,16 +1012,19 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2.5</v>
       </c>
@@ -1002,13 +1032,16 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1019,13 +1052,16 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1036,16 +1072,19 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2.6</v>
       </c>
@@ -1053,13 +1092,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1070,13 +1112,16 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1087,13 +1132,16 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1104,13 +1152,16 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1121,16 +1172,19 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2.8</v>
       </c>
@@ -1138,13 +1192,16 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1155,13 +1212,13 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1172,13 +1229,13 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1189,13 +1246,13 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1206,13 +1263,13 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1223,13 +1280,13 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1240,13 +1297,13 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1257,13 +1314,13 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1274,13 +1331,13 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1291,13 +1348,13 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1308,13 +1365,13 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1325,13 +1382,13 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1342,13 +1399,13 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>